<commit_message>
chapter 6 expample 6
</commit_message>
<xml_diff>
--- a/src/Chapter-6/案例06 批量制作数据透视表/商品销售表.xlsx
+++ b/src/Chapter-6/案例06 批量制作数据透视表/商品销售表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\example\05\为一个工作簿的工作表批量制作数据透视表\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MGF\Documents\GitHub\TianXiaPy\PyExcel\src\Chapter-6\案例06 批量制作数据透视表\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9157B02-0D66-45E9-9B2E-24AE0098FA2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB79396-B3C7-495E-B9D2-AC51FCBB8245}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1月" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="5月" sheetId="8" r:id="rId5"/>
     <sheet name="6月" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="46">
   <si>
     <t>销售日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -167,13 +167,44 @@
   <si>
     <t>2019/6/31</t>
   </si>
+  <si>
+    <t>销售地区</t>
+  </si>
+  <si>
+    <t>销售一分部</t>
+  </si>
+  <si>
+    <t>销售三分部</t>
+  </si>
+  <si>
+    <t>销售二分部</t>
+  </si>
+  <si>
+    <t>销售四分部</t>
+  </si>
+  <si>
+    <t>总计</t>
+  </si>
+  <si>
+    <t>华东</t>
+  </si>
+  <si>
+    <t>华中</t>
+  </si>
+  <si>
+    <t>华北</t>
+  </si>
+  <si>
+    <t>华南</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="5" formatCode="&quot;¥&quot;#,##0;&quot;¥&quot;\-#,##0"/>
+    <numFmt numFmtId="7" formatCode="&quot;¥&quot;#,##0.00;&quot;¥&quot;\-#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -234,7 +265,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -254,6 +285,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="5" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -536,7 +570,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
@@ -554,7 +588,7 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -579,8 +613,26 @@
       <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>43466</v>
       </c>
@@ -605,8 +657,26 @@
       <c r="H2" s="6">
         <v>616000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <v>2059200</v>
+      </c>
+      <c r="M2" s="7">
+        <v>4183800</v>
+      </c>
+      <c r="N2" s="7">
+        <v>3513200</v>
+      </c>
+      <c r="O2" s="7">
+        <v>9756200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>43466</v>
       </c>
@@ -631,8 +701,26 @@
       <c r="H3" s="6">
         <v>1310400</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="7">
+        <v>3826000</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1806200</v>
+      </c>
+      <c r="M3" s="7">
+        <v>6324000</v>
+      </c>
+      <c r="N3" s="7">
+        <v>1284000</v>
+      </c>
+      <c r="O3" s="7">
+        <v>13240200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>43467</v>
       </c>
@@ -657,8 +745,26 @@
       <c r="H4" s="6">
         <v>1190000</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="7">
+        <v>3676400</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1694000</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1245200</v>
+      </c>
+      <c r="N4" s="7">
+        <v>2552800</v>
+      </c>
+      <c r="O4" s="7">
+        <v>9168400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>43469</v>
       </c>
@@ -683,8 +789,26 @@
       <c r="H5" s="6">
         <v>778800</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="7">
+        <v>3025200</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1634600</v>
+      </c>
+      <c r="M5" s="7">
+        <v>588000</v>
+      </c>
+      <c r="N5" s="7">
+        <v>3369400</v>
+      </c>
+      <c r="O5" s="7">
+        <v>8617200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>43469</v>
       </c>
@@ -709,8 +833,26 @@
       <c r="H6" s="6">
         <v>1746000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="7">
+        <v>10527600</v>
+      </c>
+      <c r="L6" s="7">
+        <v>7194000</v>
+      </c>
+      <c r="M6" s="7">
+        <v>12341000</v>
+      </c>
+      <c r="N6" s="7">
+        <v>10719400</v>
+      </c>
+      <c r="O6" s="7">
+        <v>40782000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>43470</v>
       </c>
@@ -736,7 +878,7 @@
         <v>1148000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>43470</v>
       </c>
@@ -762,7 +904,7 @@
         <v>1831200</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>43471</v>
       </c>
@@ -788,7 +930,7 @@
         <v>272800</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>43472</v>
       </c>
@@ -814,7 +956,7 @@
         <v>720000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>43472</v>
       </c>
@@ -840,7 +982,7 @@
         <v>980000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>43473</v>
       </c>
@@ -866,7 +1008,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>43474</v>
       </c>
@@ -892,7 +1034,7 @@
         <v>1364000</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>43474</v>
       </c>
@@ -918,7 +1060,7 @@
         <v>1033200</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>43475</v>
       </c>
@@ -944,7 +1086,7 @@
         <v>828800</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>43476</v>
       </c>
@@ -1655,7 +1797,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E952D2-F0F1-4E5D-BB14-258CF9AADE6B}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -1673,7 +1815,7 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1698,8 +1840,26 @@
       <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>43497</v>
       </c>
@@ -1724,8 +1884,26 @@
       <c r="H2" s="6">
         <v>616000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <v>2072800</v>
+      </c>
+      <c r="M2" s="7">
+        <v>4531800</v>
+      </c>
+      <c r="N2" s="7">
+        <v>3994800</v>
+      </c>
+      <c r="O2" s="7">
+        <v>10599400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>43497</v>
       </c>
@@ -1750,8 +1928,26 @@
       <c r="H3" s="6">
         <v>1310400</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="7">
+        <v>4690000</v>
+      </c>
+      <c r="L3" s="7">
+        <v>2497000</v>
+      </c>
+      <c r="M3" s="7">
+        <v>2926800</v>
+      </c>
+      <c r="N3" s="7">
+        <v>2580000</v>
+      </c>
+      <c r="O3" s="7">
+        <v>12693800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>43498</v>
       </c>
@@ -1776,8 +1972,26 @@
       <c r="H4" s="6">
         <v>1190000</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="7">
+        <v>2232000</v>
+      </c>
+      <c r="L4" s="7">
+        <v>714000</v>
+      </c>
+      <c r="M4" s="7">
+        <v>2300400</v>
+      </c>
+      <c r="N4" s="7">
+        <v>3973400</v>
+      </c>
+      <c r="O4" s="7">
+        <v>9219800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>43500</v>
       </c>
@@ -1802,8 +2016,26 @@
       <c r="H5" s="6">
         <v>778800</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="7">
+        <v>4538400</v>
+      </c>
+      <c r="L5" s="7">
+        <v>583000</v>
+      </c>
+      <c r="M5" s="7">
+        <v>588000</v>
+      </c>
+      <c r="N5" s="7">
+        <v>2559600</v>
+      </c>
+      <c r="O5" s="7">
+        <v>8269000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>43500</v>
       </c>
@@ -1828,8 +2060,26 @@
       <c r="H6" s="6">
         <v>1746000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="7">
+        <v>11460400</v>
+      </c>
+      <c r="L6" s="7">
+        <v>5866800</v>
+      </c>
+      <c r="M6" s="7">
+        <v>10347000</v>
+      </c>
+      <c r="N6" s="7">
+        <v>13107800</v>
+      </c>
+      <c r="O6" s="7">
+        <v>40782000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>43501</v>
       </c>
@@ -1855,7 +2105,7 @@
         <v>1148000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>43501</v>
       </c>
@@ -1881,7 +2131,7 @@
         <v>1831200</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>43502</v>
       </c>
@@ -1907,7 +2157,7 @@
         <v>272800</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>43503</v>
       </c>
@@ -1933,7 +2183,7 @@
         <v>720000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>43503</v>
       </c>
@@ -1959,7 +2209,7 @@
         <v>980000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>43504</v>
       </c>
@@ -1985,7 +2235,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>43505</v>
       </c>
@@ -2011,7 +2261,7 @@
         <v>1364000</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>43505</v>
       </c>
@@ -2037,7 +2287,7 @@
         <v>1033200</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>43506</v>
       </c>
@@ -2063,7 +2313,7 @@
         <v>828800</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>43507</v>
       </c>
@@ -2774,7 +3024,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2391D588-A1A6-4033-804D-0A730A5720B3}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -2792,7 +3042,7 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2817,8 +3067,26 @@
       <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>43525</v>
       </c>
@@ -2843,8 +3111,26 @@
       <c r="H2" s="6">
         <v>616000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <v>2059200</v>
+      </c>
+      <c r="M2" s="7">
+        <v>4183800</v>
+      </c>
+      <c r="N2" s="7">
+        <v>3513200</v>
+      </c>
+      <c r="O2" s="7">
+        <v>9756200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>43525</v>
       </c>
@@ -2869,8 +3155,26 @@
       <c r="H3" s="6">
         <v>1310400</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="7">
+        <v>3826000</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1806200</v>
+      </c>
+      <c r="M3" s="7">
+        <v>6324000</v>
+      </c>
+      <c r="N3" s="7">
+        <v>1284000</v>
+      </c>
+      <c r="O3" s="7">
+        <v>13240200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>43526</v>
       </c>
@@ -2895,8 +3199,26 @@
       <c r="H4" s="6">
         <v>1190000</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="7">
+        <v>3676400</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1694000</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1245200</v>
+      </c>
+      <c r="N4" s="7">
+        <v>2552800</v>
+      </c>
+      <c r="O4" s="7">
+        <v>9168400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>43528</v>
       </c>
@@ -2921,8 +3243,26 @@
       <c r="H5" s="6">
         <v>778800</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="7">
+        <v>3025200</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1634600</v>
+      </c>
+      <c r="M5" s="7">
+        <v>588000</v>
+      </c>
+      <c r="N5" s="7">
+        <v>3369400</v>
+      </c>
+      <c r="O5" s="7">
+        <v>8617200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>43528</v>
       </c>
@@ -2947,8 +3287,26 @@
       <c r="H6" s="6">
         <v>1746000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="7">
+        <v>10527600</v>
+      </c>
+      <c r="L6" s="7">
+        <v>7194000</v>
+      </c>
+      <c r="M6" s="7">
+        <v>12341000</v>
+      </c>
+      <c r="N6" s="7">
+        <v>10719400</v>
+      </c>
+      <c r="O6" s="7">
+        <v>40782000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>43529</v>
       </c>
@@ -2974,7 +3332,7 @@
         <v>1148000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>43529</v>
       </c>
@@ -3000,7 +3358,7 @@
         <v>1831200</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>43530</v>
       </c>
@@ -3026,7 +3384,7 @@
         <v>272800</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>43531</v>
       </c>
@@ -3052,7 +3410,7 @@
         <v>720000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>43531</v>
       </c>
@@ -3078,7 +3436,7 @@
         <v>980000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>43532</v>
       </c>
@@ -3104,7 +3462,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>43533</v>
       </c>
@@ -3130,7 +3488,7 @@
         <v>1364000</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>43533</v>
       </c>
@@ -3156,7 +3514,7 @@
         <v>1033200</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>43534</v>
       </c>
@@ -3182,7 +3540,7 @@
         <v>828800</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>43535</v>
       </c>
@@ -3893,7 +4251,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B681D8A7-D1C2-40A3-843D-F034841F4145}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
@@ -3911,7 +4269,7 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3936,8 +4294,26 @@
       <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>43556</v>
       </c>
@@ -3962,8 +4338,26 @@
       <c r="H2" s="6">
         <v>616000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <v>3196600</v>
+      </c>
+      <c r="M2" s="7">
+        <v>2024400</v>
+      </c>
+      <c r="N2" s="7">
+        <v>4398800</v>
+      </c>
+      <c r="O2" s="7">
+        <v>9619800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>43556</v>
       </c>
@@ -3988,8 +4382,26 @@
       <c r="H3" s="6">
         <v>1310400</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="7">
+        <v>5493200</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1056000</v>
+      </c>
+      <c r="M3" s="7">
+        <v>8130200</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="7">
+        <v>14679400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>43557</v>
       </c>
@@ -4014,8 +4426,26 @@
       <c r="H4" s="6">
         <v>1190000</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="7">
+        <v>3017600</v>
+      </c>
+      <c r="L4" s="7">
+        <v>980000</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1542200</v>
+      </c>
+      <c r="N4" s="7">
+        <v>2197600</v>
+      </c>
+      <c r="O4" s="7">
+        <v>7737400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>43559</v>
       </c>
@@ -4040,8 +4470,26 @@
       <c r="H5" s="6">
         <v>778800</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="7">
+        <v>2595600</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1051600</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="7">
+        <v>4438200</v>
+      </c>
+      <c r="O5" s="7">
+        <v>8085400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>43559</v>
       </c>
@@ -4066,8 +4514,26 @@
       <c r="H6" s="6">
         <v>1746000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="7">
+        <v>11106400</v>
+      </c>
+      <c r="L6" s="7">
+        <v>6284200</v>
+      </c>
+      <c r="M6" s="7">
+        <v>11696800</v>
+      </c>
+      <c r="N6" s="7">
+        <v>11034600</v>
+      </c>
+      <c r="O6" s="7">
+        <v>40122000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>43560</v>
       </c>
@@ -4093,7 +4559,7 @@
         <v>1148000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>43560</v>
       </c>
@@ -4119,7 +4585,7 @@
         <v>1831200</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>43561</v>
       </c>
@@ -4145,7 +4611,7 @@
         <v>272800</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>43562</v>
       </c>
@@ -4171,7 +4637,7 @@
         <v>720000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>43562</v>
       </c>
@@ -4197,7 +4663,7 @@
         <v>980000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>43563</v>
       </c>
@@ -4223,7 +4689,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>43564</v>
       </c>
@@ -4249,7 +4715,7 @@
         <v>1364000</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>43564</v>
       </c>
@@ -4275,7 +4741,7 @@
         <v>1033200</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>43565</v>
       </c>
@@ -4301,7 +4767,7 @@
         <v>828800</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>43566</v>
       </c>
@@ -5016,7 +5482,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BBF2BA6-A9B6-445F-B1D6-6DFEB6617E58}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -5034,7 +5500,7 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5059,8 +5525,26 @@
       <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>43586</v>
       </c>
@@ -5085,8 +5569,26 @@
       <c r="H2" s="6">
         <v>616000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <v>2059200</v>
+      </c>
+      <c r="M2" s="7">
+        <v>4183800</v>
+      </c>
+      <c r="N2" s="7">
+        <v>3513200</v>
+      </c>
+      <c r="O2" s="7">
+        <v>9756200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>43586</v>
       </c>
@@ -5111,8 +5613,26 @@
       <c r="H3" s="6">
         <v>1310400</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="7">
+        <v>3826000</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1806200</v>
+      </c>
+      <c r="M3" s="7">
+        <v>6324000</v>
+      </c>
+      <c r="N3" s="7">
+        <v>1284000</v>
+      </c>
+      <c r="O3" s="7">
+        <v>13240200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>43587</v>
       </c>
@@ -5137,8 +5657,26 @@
       <c r="H4" s="6">
         <v>1190000</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="7">
+        <v>3676400</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1694000</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1245200</v>
+      </c>
+      <c r="N4" s="7">
+        <v>2552800</v>
+      </c>
+      <c r="O4" s="7">
+        <v>9168400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>43589</v>
       </c>
@@ -5163,8 +5701,26 @@
       <c r="H5" s="6">
         <v>778800</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="7">
+        <v>3025200</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1634600</v>
+      </c>
+      <c r="M5" s="7">
+        <v>588000</v>
+      </c>
+      <c r="N5" s="7">
+        <v>3369400</v>
+      </c>
+      <c r="O5" s="7">
+        <v>8617200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>43589</v>
       </c>
@@ -5189,8 +5745,26 @@
       <c r="H6" s="6">
         <v>1746000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="7">
+        <v>10527600</v>
+      </c>
+      <c r="L6" s="7">
+        <v>7194000</v>
+      </c>
+      <c r="M6" s="7">
+        <v>12341000</v>
+      </c>
+      <c r="N6" s="7">
+        <v>10719400</v>
+      </c>
+      <c r="O6" s="7">
+        <v>40782000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>43590</v>
       </c>
@@ -5216,7 +5790,7 @@
         <v>1148000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>43590</v>
       </c>
@@ -5242,7 +5816,7 @@
         <v>1831200</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>43591</v>
       </c>
@@ -5268,7 +5842,7 @@
         <v>272800</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>43592</v>
       </c>
@@ -5294,7 +5868,7 @@
         <v>720000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>43592</v>
       </c>
@@ -5320,7 +5894,7 @@
         <v>980000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>43593</v>
       </c>
@@ -5346,7 +5920,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>43594</v>
       </c>
@@ -5372,7 +5946,7 @@
         <v>1364000</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>43594</v>
       </c>
@@ -5398,7 +5972,7 @@
         <v>1033200</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>43595</v>
       </c>
@@ -5424,7 +5998,7 @@
         <v>828800</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>43596</v>
       </c>
@@ -6135,7 +6709,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015DD46E-4C56-48C6-B33E-CFC7D889022F}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -6153,7 +6727,7 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6178,8 +6752,26 @@
       <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>43617</v>
       </c>
@@ -6204,8 +6796,26 @@
       <c r="H2" s="6">
         <v>616000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <v>2059200</v>
+      </c>
+      <c r="M2" s="7">
+        <v>4183800</v>
+      </c>
+      <c r="N2" s="7">
+        <v>3513200</v>
+      </c>
+      <c r="O2" s="7">
+        <v>9756200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>43617</v>
       </c>
@@ -6230,8 +6840,26 @@
       <c r="H3" s="6">
         <v>1310400</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="7">
+        <v>3826000</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1806200</v>
+      </c>
+      <c r="M3" s="7">
+        <v>6324000</v>
+      </c>
+      <c r="N3" s="7">
+        <v>1284000</v>
+      </c>
+      <c r="O3" s="7">
+        <v>13240200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>43618</v>
       </c>
@@ -6256,8 +6884,26 @@
       <c r="H4" s="6">
         <v>1190000</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="7">
+        <v>3676400</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1694000</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1245200</v>
+      </c>
+      <c r="N4" s="7">
+        <v>2552800</v>
+      </c>
+      <c r="O4" s="7">
+        <v>9168400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>43620</v>
       </c>
@@ -6282,8 +6928,26 @@
       <c r="H5" s="6">
         <v>778800</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="7">
+        <v>3025200</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1634600</v>
+      </c>
+      <c r="M5" s="7">
+        <v>588000</v>
+      </c>
+      <c r="N5" s="7">
+        <v>3369400</v>
+      </c>
+      <c r="O5" s="7">
+        <v>8617200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>43620</v>
       </c>
@@ -6308,8 +6972,26 @@
       <c r="H6" s="6">
         <v>1746000</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="J6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="7">
+        <v>10527600</v>
+      </c>
+      <c r="L6" s="7">
+        <v>7194000</v>
+      </c>
+      <c r="M6" s="7">
+        <v>12341000</v>
+      </c>
+      <c r="N6" s="7">
+        <v>10719400</v>
+      </c>
+      <c r="O6" s="7">
+        <v>40782000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>43621</v>
       </c>
@@ -6335,7 +7017,7 @@
         <v>1148000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>43621</v>
       </c>
@@ -6361,7 +7043,7 @@
         <v>1831200</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>43622</v>
       </c>
@@ -6387,7 +7069,7 @@
         <v>272800</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>43623</v>
       </c>
@@ -6413,7 +7095,7 @@
         <v>720000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>43623</v>
       </c>
@@ -6439,7 +7121,7 @@
         <v>980000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>43624</v>
       </c>
@@ -6465,7 +7147,7 @@
         <v>1800000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>43625</v>
       </c>
@@ -6491,7 +7173,7 @@
         <v>1364000</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>43625</v>
       </c>
@@ -6517,7 +7199,7 @@
         <v>1033200</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>43626</v>
       </c>
@@ -6543,7 +7225,7 @@
         <v>828800</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>43627</v>
       </c>

</xml_diff>